<commit_message>
Fixed bug where endpoints were incorrectly selected for squares where one is inside the other
</commit_message>
<xml_diff>
--- a/Java/Chapter 7/Question7_5/Square Cut Tester - Chapter 10, Problem 5.xlsx
+++ b/Java/Chapter 7/Question7_5/Square Cut Tester - Chapter 10, Problem 5.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="5955"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diagram" sheetId="1" r:id="rId1"/>
+    <sheet name="Square" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>Square 1</t>
   </si>
@@ -38,6 +39,15 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
 </sst>
 </file>
@@ -296,48 +306,48 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Diagram!$B$8:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$6</c:f>
+              <c:f>Diagram!$C$8:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -352,48 +362,48 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$B$11</c:f>
+              <c:f>Diagram!$B$13:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$11</c:f>
+              <c:f>Diagram!$C$13:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -405,7 +415,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$14</c:f>
+              <c:f>Diagram!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -416,24 +426,24 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$14</c:f>
+              <c:f>Diagram!$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14</c:f>
+              <c:f>Diagram!$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -445,7 +455,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Diagram!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -456,24 +466,24 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$15</c:f>
+              <c:f>Diagram!$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$15</c:f>
+              <c:f>Diagram!$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.5</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -488,7 +498,22 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$13</c:f>
+              <c:f>Diagram!$B$4:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Diagram!$C$4:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -496,22 +521,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$12:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -526,11 +536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42418944"/>
-        <c:axId val="42300544"/>
+        <c:axId val="62221312"/>
+        <c:axId val="62223104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42418944"/>
+        <c:axId val="62221312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -540,12 +550,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42300544"/>
+        <c:crossAx val="62223104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42300544"/>
+        <c:axId val="62223104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42418944"/>
+        <c:crossAx val="62221312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -582,16 +592,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>147636</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -900,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,173 +922,238 @@
     <col min="2" max="3" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>23</v>
+      </c>
+      <c r="C4" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B8" s="3">
+        <f>Diagram!B2</f>
+        <v>10</v>
+      </c>
+      <c r="C8" s="3">
+        <f>Diagram!C2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B8</f>
+        <v>10</v>
+      </c>
+      <c r="C9" s="10">
+        <f>C8+Diagram!D2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B9+Diagram!D2</f>
+        <v>20</v>
+      </c>
+      <c r="C10" s="10">
+        <f>C9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
+        <f>B10</f>
+        <v>20</v>
+      </c>
+      <c r="C11" s="10">
+        <f>C10-Diagram!D2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4">
+        <f>B8</f>
+        <v>10</v>
+      </c>
+      <c r="C12" s="12">
+        <f>C8</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3">
+        <f>Diagram!B3</f>
+        <v>8</v>
+      </c>
+      <c r="C13" s="3">
+        <f>Diagram!C3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="C14" s="10">
+        <f>C13+Diagram!D3</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3">
+        <f>B14+Diagram!D3</f>
+        <v>23</v>
+      </c>
+      <c r="C15" s="10">
+        <f>C14</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <f>B15</f>
+        <v>23</v>
+      </c>
+      <c r="C16" s="10">
+        <f>C15-Diagram!D3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4">
+        <f>B13</f>
+        <v>8</v>
+      </c>
+      <c r="C17" s="12">
+        <f>C13</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3">
+        <f>(MAX(B8:B12)+MIN(B8:B12))/2</f>
+        <v>15</v>
+      </c>
+      <c r="C20" s="10">
+        <f>(MAX(C8:C12)+MIN(C8:C12))/2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3">
-        <v>7</v>
-      </c>
-      <c r="C3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3">
-        <v>7</v>
-      </c>
-      <c r="C4" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="3">
-        <v>4</v>
-      </c>
-      <c r="C5" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5">
-        <v>7</v>
-      </c>
-      <c r="C12" s="14">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3">
-        <f>(MAX(B2:B6)+MIN(B2:B6))/2</f>
-        <v>5.5</v>
-      </c>
-      <c r="C14" s="10">
-        <f>(MAX(C2:C6)+MIN(C2:C6))/2</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4">
-        <f>(MAX(B7:B11)+MIN(B7:B11))/2</f>
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="12">
-        <f>(MAX(C7:C11)+MIN(C7:C11))/2</f>
-        <v>4.5</v>
+      <c r="B21" s="4">
+        <f>(MAX(B13:B17)+MIN(B13:B17))/2</f>
+        <v>15.5</v>
+      </c>
+      <c r="C21" s="12">
+        <f>(MAX(C13:C17)+MIN(C13:C17))/2</f>
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>
@@ -1086,4 +1161,18 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>